<commit_message>
Comentarios de introducir Actualizada hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="53">
   <si>
     <t>GP</t>
   </si>
@@ -479,12 +479,21 @@
   <si>
     <t>Reunion con el profesor: auditoria externa</t>
   </si>
+  <si>
+    <t>Reuncion para preparar la presentacion</t>
+  </si>
+  <si>
+    <t>Ahora se pueden introducir modelos a traves de la aplicación</t>
+  </si>
+  <si>
+    <t>Introducidos varios modelos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -562,6 +571,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1247,7 +1262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1417,23 +1432,39 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCCFFFF"/>
           <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
         </patternFill>
       </fill>
       <border>
@@ -1474,50 +1505,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFCCFFFF"/>
           <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
         </patternFill>
       </fill>
       <border>
@@ -1981,7 +1970,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2079,11 +2068,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111977216"/>
-        <c:axId val="111979136"/>
+        <c:axId val="122796288"/>
+        <c:axId val="122810752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111977216"/>
+        <c:axId val="122796288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,7 +2112,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111979136"/>
+        <c:crossAx val="122810752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2131,7 +2120,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111979136"/>
+        <c:axId val="122810752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2175,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111977216"/>
+        <c:crossAx val="122796288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2262,6 +2251,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2283,6 +2315,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4098" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2358,6 +2433,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2379,6 +2497,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2050" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2479,6 +2640,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2500,6 +2704,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2575,6 +2822,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2596,6 +2886,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8194" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2671,6 +3004,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2692,6 +3068,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10242" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2767,6 +3186,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2788,6 +3250,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3074" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3166,8 +3671,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -5775,12 +6280,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5852,8 +6357,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -8609,12 +9114,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8685,8 +9190,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="131"/>
-      <c r="AR1" s="132"/>
+      <c r="AQ1" s="133"/>
+      <c r="AR1" s="134"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -11394,12 +11899,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11471,8 +11976,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -14228,12 +14733,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14456,7 +14961,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>22.9</v>
+        <v>25.65</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -14476,7 +14981,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -15583,12 +16088,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15656,8 +16161,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="131"/>
-      <c r="AP1" s="132"/>
+      <c r="AO1" s="133"/>
+      <c r="AP1" s="134"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="3"/>
       <c r="AS1" s="3"/>
@@ -18265,12 +18770,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18342,8 +18847,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -21126,12 +21631,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21202,8 +21707,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="131"/>
-      <c r="AR1" s="132"/>
+      <c r="AQ1" s="133"/>
+      <c r="AR1" s="134"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -23940,12 +24445,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23960,7 +24465,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24019,8 +24524,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -24183,7 +24688,7 @@
         <v>48</v>
       </c>
       <c r="G3" s="46">
-        <f t="shared" ref="G3:G4" si="0">SUM(H3:AL3)</f>
+        <f t="shared" ref="G3" si="0">SUM(H3:AL3)</f>
         <v>1</v>
       </c>
       <c r="H3" s="26"/>
@@ -24242,13 +24747,13 @@
       <c r="B4" s="22">
         <v>84</v>
       </c>
-      <c r="C4" s="133">
+      <c r="C4" s="131">
         <v>2</v>
       </c>
       <c r="D4" s="23">
         <v>44</v>
       </c>
-      <c r="E4" s="134">
+      <c r="E4" s="132">
         <v>0</v>
       </c>
       <c r="F4" s="15" t="s">
@@ -24311,14 +24816,24 @@
     </row>
     <row r="5" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="22">
+        <v>84</v>
+      </c>
+      <c r="C5" s="23">
+        <v>2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>58</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="G5" s="16">
-        <f t="shared" ref="G3:G36" si="2">SUM(H5:AL5)</f>
-        <v>0</v>
+        <f t="shared" ref="G5:G36" si="2">SUM(H5:AL5)</f>
+        <v>1</v>
       </c>
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
@@ -24333,7 +24848,9 @@
       <c r="R5" s="23"/>
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
+      <c r="U5" s="23">
+        <v>1</v>
+      </c>
       <c r="V5" s="23"/>
       <c r="W5" s="26"/>
       <c r="X5" s="26"/>
@@ -24371,14 +24888,24 @@
     </row>
     <row r="6" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="22">
+        <v>84</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>55</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -24393,7 +24920,9 @@
       <c r="R6" s="23"/>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
+      <c r="U6" s="23">
+        <v>1.5</v>
+      </c>
       <c r="V6" s="23"/>
       <c r="W6" s="26"/>
       <c r="X6" s="26"/>
@@ -24431,14 +24960,24 @@
     </row>
     <row r="7" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="16">
+      <c r="B7" s="22">
+        <v>84</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2</v>
+      </c>
+      <c r="D7" s="23">
+        <v>55</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+      <c r="F7" s="136" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -24453,8 +24992,10 @@
       <c r="R7" s="23"/>
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
+      <c r="U7" s="135"/>
+      <c r="V7" s="135">
+        <v>0.25</v>
+      </c>
       <c r="W7" s="26"/>
       <c r="X7" s="26"/>
       <c r="Y7" s="23"/>
@@ -26180,7 +26721,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -26236,11 +26777,11 @@
       </c>
       <c r="U36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="V36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="W36" s="78">
         <f t="shared" si="3"/>
@@ -26741,38 +27282,39 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:G35">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G35">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -26837,8 +27379,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="131"/>
-      <c r="AR1" s="132"/>
+      <c r="AQ1" s="133"/>
+      <c r="AR1" s="134"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -29490,12 +30032,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29568,8 +30110,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -32268,12 +32810,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32345,8 +32887,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="131"/>
-      <c r="AS1" s="132"/>
+      <c r="AR1" s="133"/>
+      <c r="AS1" s="134"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -35045,12 +35587,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35121,8 +35663,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="131"/>
-      <c r="AR1" s="132"/>
+      <c r="AQ1" s="133"/>
+      <c r="AR1" s="134"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -37774,12 +38316,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Funcionalidad: Ordenar listado de coches por modelo. Actualizada hoja de calculo
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="54">
   <si>
     <t>GP</t>
   </si>
@@ -487,6 +487,9 @@
   </si>
   <si>
     <t>Introducidos varios modelos</t>
+  </si>
+  <si>
+    <t>Funcionalidad: Ordenar lista de coches por modelo</t>
   </si>
 </sst>
 </file>
@@ -1434,46 +1437,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1970,7 +1945,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.75</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2068,11 +2043,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122796288"/>
-        <c:axId val="122810752"/>
+        <c:axId val="60824576"/>
+        <c:axId val="60830848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122796288"/>
+        <c:axId val="60824576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2112,7 +2087,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122810752"/>
+        <c:crossAx val="60830848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2120,7 +2095,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122810752"/>
+        <c:axId val="60830848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2150,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122796288"/>
+        <c:crossAx val="60824576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2294,6 +2269,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2358,6 +2376,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2476,6 +2537,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2540,6 +2644,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2683,6 +2830,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2747,6 +2937,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2865,6 +3098,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2929,6 +3205,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3047,6 +3366,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3111,6 +3473,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3229,6 +3634,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3293,6 +3741,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3671,8 +4162,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -6280,12 +6771,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6357,8 +6848,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -9114,12 +9605,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9190,8 +9681,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="133"/>
-      <c r="AR1" s="134"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="136"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -11899,12 +12390,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11976,8 +12467,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -14733,12 +15224,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14961,7 +15452,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>25.65</v>
+        <v>26.4</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -14981,7 +15472,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -16088,12 +16579,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16161,8 +16652,8 @@
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="133"/>
-      <c r="AP1" s="134"/>
+      <c r="AO1" s="135"/>
+      <c r="AP1" s="136"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="3"/>
       <c r="AS1" s="3"/>
@@ -18770,12 +19261,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18847,8 +19338,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -21631,12 +22122,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21707,8 +22198,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="133"/>
-      <c r="AR1" s="134"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="136"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -24445,12 +24936,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24465,7 +24956,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24524,8 +25015,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -24972,7 +25463,7 @@
       <c r="E7" s="24">
         <v>0</v>
       </c>
-      <c r="F7" s="136" t="s">
+      <c r="F7" s="134" t="s">
         <v>52</v>
       </c>
       <c r="G7" s="46">
@@ -24992,8 +25483,8 @@
       <c r="R7" s="23"/>
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
-      <c r="U7" s="135"/>
-      <c r="V7" s="135">
+      <c r="U7" s="133"/>
+      <c r="V7" s="133">
         <v>0.25</v>
       </c>
       <c r="W7" s="26"/>
@@ -25032,14 +25523,24 @@
     </row>
     <row r="8" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="22">
+        <v>84</v>
+      </c>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
+      <c r="D8" s="23">
+        <v>54</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>53</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -25055,7 +25556,9 @@
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
+      <c r="V8" s="23">
+        <v>0.75</v>
+      </c>
       <c r="W8" s="26"/>
       <c r="X8" s="26"/>
       <c r="Y8" s="23"/>
@@ -26721,7 +27224,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -26781,7 +27284,7 @@
       </c>
       <c r="V36" s="79">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="W36" s="78">
         <f t="shared" si="3"/>
@@ -27282,32 +27785,32 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:G35">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G35">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27379,8 +27882,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="133"/>
-      <c r="AR1" s="134"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="136"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -30032,12 +30535,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30110,8 +30613,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -32810,12 +33313,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32887,8 +33390,8 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="133"/>
-      <c r="AS1" s="134"/>
+      <c r="AR1" s="135"/>
+      <c r="AS1" s="136"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="3"/>
       <c r="AV1" s="3"/>
@@ -35587,12 +36090,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35663,8 +36166,8 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
-      <c r="AQ1" s="133"/>
-      <c r="AR1" s="134"/>
+      <c r="AQ1" s="135"/>
+      <c r="AR1" s="136"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="3"/>
       <c r="AU1" s="3"/>
@@ -38316,12 +38819,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Añadidas unidades a los filtros (€, CV, l/100km) Corregido error al ordenar por modelo Actualizada hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="55">
   <si>
     <t>GP</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Funcionalidad: Ordenar lista de coches por modelo</t>
+  </si>
+  <si>
+    <t>Corregidos errores de unidades y ordenacion</t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1948,7 @@
                   <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2043,11 +2046,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="60824576"/>
-        <c:axId val="60830848"/>
+        <c:axId val="63856640"/>
+        <c:axId val="63858560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60824576"/>
+        <c:axId val="63856640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +2090,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60830848"/>
+        <c:crossAx val="63858560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2095,7 +2098,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60830848"/>
+        <c:axId val="63858560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,7 +2153,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60824576"/>
+        <c:crossAx val="63856640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2312,6 +2315,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2419,6 +2465,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2580,6 +2669,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2687,6 +2819,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2873,6 +3048,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2980,6 +3198,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3141,6 +3402,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3248,6 +3552,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3409,6 +3756,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3516,6 +3906,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3677,6 +4110,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3784,6 +4260,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -15452,7 +15971,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>26.4</v>
+        <v>26.599999999999998</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -15472,7 +15991,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -24956,7 +25475,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -25595,14 +26114,24 @@
     </row>
     <row r="9" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="22">
+        <v>84</v>
+      </c>
+      <c r="C9" s="23">
+        <v>2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>55</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -25618,7 +26147,9 @@
       <c r="S9" s="23"/>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
+      <c r="V9" s="23">
+        <v>0.2</v>
+      </c>
       <c r="W9" s="26"/>
       <c r="X9" s="26"/>
       <c r="Y9" s="23"/>
@@ -27224,7 +27755,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -27284,7 +27815,7 @@
       </c>
       <c r="V36" s="79">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="W36" s="78">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Actualizada hoja de esfuerzos y de equipo
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="56">
   <si>
     <t>GP</t>
   </si>
@@ -480,9 +480,6 @@
     <t>Reunion con el profesor: auditoria externa</t>
   </si>
   <si>
-    <t>Reuncion para preparar la presentacion</t>
-  </si>
-  <si>
     <t>Ahora se pueden introducir modelos a traves de la aplicación</t>
   </si>
   <si>
@@ -493,6 +490,12 @@
   </si>
   <si>
     <t>Ordenacion de modelos mediante todos los campos de un modelo(ascendente y descendente)</t>
+  </si>
+  <si>
+    <t>Reunion para preparar la presentacion</t>
+  </si>
+  <si>
+    <t>Reunion para preparar la presentacion tecnica y reparto de tareas</t>
   </si>
 </sst>
 </file>
@@ -1451,35 +1454,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1965,6 +1940,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2002,10 +1978,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.5</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2103,11 +2079,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73340416"/>
-        <c:axId val="73342336"/>
+        <c:axId val="49452928"/>
+        <c:axId val="49467392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73340416"/>
+        <c:axId val="49452928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,6 +2109,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="cross"/>
@@ -2148,7 +2125,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73342336"/>
+        <c:crossAx val="49467392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2156,7 +2133,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73342336"/>
+        <c:axId val="49467392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,6 +2168,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2212,7 +2190,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73340416"/>
+        <c:crossAx val="49452928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,6 +2202,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2476,6 +2455,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2766,6 +2831,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3029,6 +3180,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3265,6 +3502,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3580,6 +3903,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3816,6 +4225,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4106,6 +4601,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4342,6 +4923,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4632,6 +5299,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4868,6 +5621,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5158,6 +5997,92 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5394,6 +6319,92 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -16853,7 +17864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17062,7 +18073,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>31.25</v>
+        <v>35.25</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -17078,11 +18089,11 @@
       </c>
       <c r="K6" s="83">
         <f>Abr!G36</f>
-        <v>9</v>
+        <v>10.75</v>
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>7.5</v>
+        <v>9.75</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -23754,7 +24765,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:AG11"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24112,8 +25123,8 @@
         <v>17</v>
       </c>
       <c r="G5" s="16">
-        <f>SUM(H5:AK5)</f>
-        <v>0.5</v>
+        <f t="shared" ref="G5:G10" si="0">SUM(H5:AK5)</f>
+        <v>1</v>
       </c>
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
@@ -24125,7 +25136,7 @@
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
       <c r="Q5" s="44">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R5" s="26"/>
       <c r="S5" s="26"/>
@@ -24183,8 +25194,8 @@
         <v>26</v>
       </c>
       <c r="G6" s="16">
-        <f>SUM(H6:AK6)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -24198,7 +25209,7 @@
       <c r="Q6" s="23"/>
       <c r="R6" s="26"/>
       <c r="S6" s="66">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
@@ -24252,7 +25263,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="16">
-        <f>SUM(H7:AK7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H7" s="26"/>
@@ -24321,7 +25332,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="16">
-        <f>SUM(H8:AK8)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="H8" s="26"/>
@@ -24390,8 +25401,8 @@
         <v>29</v>
       </c>
       <c r="G9" s="16">
-        <f>SUM(H9:AK9)</f>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -24412,7 +25423,7 @@
       <c r="X9" s="23"/>
       <c r="Y9" s="26"/>
       <c r="Z9" s="66">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
@@ -24461,8 +25472,8 @@
         <v>30</v>
       </c>
       <c r="G10" s="16">
-        <f>SUM(H10:AK10)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -24489,7 +25500,7 @@
       <c r="AD10" s="26"/>
       <c r="AE10" s="26"/>
       <c r="AF10" s="66">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AG10" s="26"/>
       <c r="AH10" s="23"/>
@@ -24546,7 +25557,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
       <c r="G12" s="16">
-        <f>SUM(H12:AK12)</f>
+        <f t="shared" ref="G12:G36" si="1">SUM(H12:AK12)</f>
         <v>0</v>
       </c>
       <c r="H12" s="26"/>
@@ -24605,7 +25616,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="16">
-        <f>SUM(H13:AK13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H13" s="26"/>
@@ -24664,7 +25675,7 @@
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="16">
-        <f>SUM(H14:AK14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14" s="26"/>
@@ -24723,7 +25734,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="16">
-        <f>SUM(H15:AK15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15" s="26"/>
@@ -24782,7 +25793,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="16">
-        <f>SUM(H16:AK16)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H16" s="26"/>
@@ -24841,7 +25852,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
       <c r="G17" s="16">
-        <f>SUM(H17:AK17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H17" s="26"/>
@@ -24900,7 +25911,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="16">
-        <f>SUM(H18:AK18)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" s="26"/>
@@ -24959,7 +25970,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="16">
-        <f>SUM(H19:AK19)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" s="26"/>
@@ -25018,7 +26029,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
       <c r="G20" s="16">
-        <f>SUM(H20:AK20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="26"/>
@@ -25077,7 +26088,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
       <c r="G21" s="16">
-        <f>SUM(H21:AK21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="26"/>
@@ -25136,7 +26147,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
       <c r="G22" s="16">
-        <f>SUM(H22:AK22)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22" s="26"/>
@@ -25195,7 +26206,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="25"/>
       <c r="G23" s="16">
-        <f>SUM(H23:AK23)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23" s="26"/>
@@ -25254,7 +26265,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="25"/>
       <c r="G24" s="16">
-        <f>SUM(H24:AK24)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24" s="26"/>
@@ -25313,7 +26324,7 @@
       <c r="E25" s="24"/>
       <c r="F25" s="25"/>
       <c r="G25" s="16">
-        <f>SUM(H25:AK25)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25" s="26"/>
@@ -25372,7 +26383,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
       <c r="G26" s="16">
-        <f>SUM(H26:AK26)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H26" s="26"/>
@@ -25431,7 +26442,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="25"/>
       <c r="G27" s="16">
-        <f>SUM(H27:AK27)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H27" s="26"/>
@@ -25490,7 +26501,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="25"/>
       <c r="G28" s="16">
-        <f>SUM(H28:AK28)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="26"/>
@@ -25549,7 +26560,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
       <c r="G29" s="16">
-        <f>SUM(H29:AK29)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H29" s="26"/>
@@ -25608,7 +26619,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
       <c r="G30" s="16">
-        <f>SUM(H30:AK30)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H30" s="26"/>
@@ -25667,7 +26678,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
       <c r="G31" s="16">
-        <f>SUM(H31:AK31)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H31" s="26"/>
@@ -25726,7 +26737,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="25"/>
       <c r="G32" s="16">
-        <f>SUM(H32:AK32)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H32" s="26"/>
@@ -25785,7 +26796,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="G33" s="16">
-        <f>SUM(H33:AK33)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H33" s="26"/>
@@ -25844,7 +26855,7 @@
       <c r="E34" s="24"/>
       <c r="F34" s="25"/>
       <c r="G34" s="16">
-        <f>SUM(H34:AK34)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H34" s="26"/>
@@ -25903,7 +26914,7 @@
       <c r="E35" s="63"/>
       <c r="F35" s="64"/>
       <c r="G35" s="16">
-        <f>SUM(H35:AK35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H35" s="69"/>
@@ -25964,127 +26975,127 @@
         <v>31</v>
       </c>
       <c r="G36" s="76">
-        <f>SUM(H36:AK36)</f>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>10.75</v>
       </c>
       <c r="H36" s="78">
-        <f>SUM(H3:H35)</f>
+        <f t="shared" ref="H36:AK36" si="2">SUM(H3:H35)</f>
         <v>0</v>
       </c>
       <c r="I36" s="78">
-        <f>SUM(I3:I35)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J36" s="78">
-        <f>SUM(J3:J35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K36" s="78">
-        <f>SUM(K3:K35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L36" s="78">
-        <f>SUM(L3:L35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M36" s="78">
-        <f>SUM(M3:M35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N36" s="79">
-        <f>SUM(N3:N35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O36" s="79">
-        <f>SUM(O3:O35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P36" s="79">
-        <f>SUM(P3:P35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q36" s="79">
-        <f>SUM(Q3:Q35)</f>
-        <v>1.5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="R36" s="78">
-        <f>SUM(R3:R35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S36" s="78">
-        <f>SUM(S3:S35)</f>
-        <v>1.5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="T36" s="79">
-        <f>SUM(T3:T35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U36" s="79">
-        <f>SUM(U3:U35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V36" s="79">
-        <f>SUM(V3:V35)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="W36" s="79">
-        <f>SUM(W3:W35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X36" s="79">
-        <f>SUM(X3:X35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y36" s="78">
-        <f>SUM(Y3:Y35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z36" s="78">
-        <f>SUM(Z3:Z35)</f>
-        <v>1.5</v>
+        <f t="shared" si="2"/>
+        <v>1.75</v>
       </c>
       <c r="AA36" s="79">
-        <f>SUM(AA3:AA35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB36" s="79">
-        <f>SUM(AB3:AB35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC36" s="79">
-        <f>SUM(AC3:AC35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD36" s="78">
-        <f>SUM(AD3:AD35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE36" s="78">
-        <f>SUM(AE3:AE35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF36" s="78">
-        <f>SUM(AF3:AF35)</f>
-        <v>1.5</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="AG36" s="78">
-        <f>SUM(AG3:AG35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH36" s="79">
-        <f>SUM(AH3:AH35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI36" s="79">
-        <f>SUM(AI3:AI35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="79">
-        <f>SUM(AJ3:AJ35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK36" s="79">
-        <f>SUM(AK3:AK35)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL36" s="1"/>
@@ -26534,8 +27545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26899,7 +27910,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" ref="G5:G36" si="2">SUM(H5:AL5)</f>
@@ -26971,7 +27982,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="16">
         <f t="shared" si="2"/>
@@ -27043,11 +28054,11 @@
         <v>0</v>
       </c>
       <c r="F7" s="134" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="46">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -27064,7 +28075,7 @@
       <c r="T7" s="23"/>
       <c r="U7" s="133"/>
       <c r="V7" s="133">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W7" s="26"/>
       <c r="X7" s="26"/>
@@ -27115,7 +28126,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="16">
         <f t="shared" si="2"/>
@@ -27187,11 +28198,11 @@
         <v>7</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="16">
         <f>SUM(H9:AG9)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -27212,7 +28223,9 @@
         <v>2</v>
       </c>
       <c r="X9" s="23"/>
-      <c r="Y9" s="26"/>
+      <c r="Y9" s="26">
+        <v>1</v>
+      </c>
       <c r="Z9" s="26"/>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
@@ -27246,14 +28259,24 @@
     </row>
     <row r="10" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="B10" s="22">
+        <v>84</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2</v>
+      </c>
+      <c r="D10" s="23">
+        <v>58</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>55</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -27272,7 +28295,9 @@
       <c r="V10" s="23"/>
       <c r="W10" s="26"/>
       <c r="X10" s="26"/>
-      <c r="Y10" s="23"/>
+      <c r="Y10" s="23">
+        <v>1</v>
+      </c>
       <c r="Z10" s="23"/>
       <c r="AA10" s="23"/>
       <c r="AB10" s="23"/>
@@ -28815,7 +29840,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>9.75</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -28875,7 +29900,7 @@
       </c>
       <c r="V36" s="79">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="W36" s="78">
         <f t="shared" si="3"/>
@@ -28887,7 +29912,7 @@
       </c>
       <c r="Y36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z36" s="79">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Manual de Usuario.doc Manual de Usuario.pdf Actualizada hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="57">
   <si>
     <t>GP</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>Reunion para preparar la presentacion tecnica y reparto de tareas</t>
+  </si>
+  <si>
+    <t>Manual de usuario</t>
   </si>
 </sst>
 </file>
@@ -1981,7 +1984,7 @@
                   <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.75</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2079,11 +2082,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49452928"/>
-        <c:axId val="49467392"/>
+        <c:axId val="96083968"/>
+        <c:axId val="96085888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49452928"/>
+        <c:axId val="96083968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2128,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49467392"/>
+        <c:crossAx val="96085888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2133,7 +2136,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49467392"/>
+        <c:axId val="96085888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2190,7 +2193,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49452928"/>
+        <c:crossAx val="96083968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2568,6 +2571,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2890,6 +2936,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3266,6 +3355,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3588,6 +3720,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3989,6 +4164,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4311,6 +4529,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4687,6 +4948,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5036,6 +5340,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5358,6 +5710,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5734,6 +6129,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6083,6 +6521,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6405,6 +6886,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -17864,7 +18388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18073,7 +18597,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>35.25</v>
+        <v>38.75</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -18093,7 +18617,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>9.75</v>
+        <v>13.25</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -27545,8 +28069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28331,14 +28855,22 @@
     </row>
     <row r="11" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="B11" s="22">
+        <v>84</v>
+      </c>
+      <c r="C11" s="23">
+        <v>2</v>
+      </c>
+      <c r="D11" s="23">
+        <v>57</v>
+      </c>
       <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="G11" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -28361,7 +28893,9 @@
       <c r="Z11" s="23"/>
       <c r="AA11" s="23"/>
       <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
+      <c r="AC11" s="23">
+        <v>3.5</v>
+      </c>
       <c r="AD11" s="26"/>
       <c r="AE11" s="26"/>
       <c r="AF11" s="23"/>
@@ -29840,7 +30374,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>9.75</v>
+        <v>13.25</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -29928,7 +30462,7 @@
       </c>
       <c r="AC36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="AD36" s="78">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Manual de Administrador.doc Manual de Administrador.pdf Actualizada hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <definedName name="Print_Area" localSheetId="8">Sep!$A$1:$AR$37</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -69,7 +70,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -88,30 +89,6 @@
 </file>
 
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="AQ2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Se anotará la autoformación en línea (foros, manuales, ejercicios,etc.) y la formación presencial (cursos, seminarios, congresos…)
-Detallar brevemente en esta columna en qué ha consistido la formación</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -213,7 +190,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +214,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -285,7 +262,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AR2" authorId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +286,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AQ2" authorId="0">
+    <comment ref="AR2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -328,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="58">
   <si>
     <t>GP</t>
   </si>
@@ -499,6 +476,9 @@
   </si>
   <si>
     <t>Manual de usuario</t>
+  </si>
+  <si>
+    <t>Manual de administrador</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +1964,7 @@
                   <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.25</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2082,11 +2062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96083968"/>
-        <c:axId val="96085888"/>
+        <c:axId val="49685632"/>
+        <c:axId val="49687552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96083968"/>
+        <c:axId val="49685632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2108,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96085888"/>
+        <c:crossAx val="49687552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2136,7 +2116,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96085888"/>
+        <c:axId val="49687552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2173,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96083968"/>
+        <c:crossAx val="49685632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2614,6 +2594,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2979,6 +3002,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3398,6 +3464,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3763,6 +3872,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4207,6 +4359,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4599,6 +4794,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4964,6 +5202,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -5780,6 +6061,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6145,6 +6469,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6564,6 +6931,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6956,6 +7366,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18597,7 +19050,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>38.75</v>
+        <v>40.75</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -18617,7 +19070,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>13.25</v>
+        <v>15.25</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -22425,7 +22878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -28066,11 +28519,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28925,14 +29378,22 @@
     </row>
     <row r="12" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="B12" s="22">
+        <v>84</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23">
+        <v>57</v>
+      </c>
       <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25" t="s">
+        <v>57</v>
+      </c>
       <c r="G12" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -28955,7 +29416,9 @@
       <c r="Z12" s="23"/>
       <c r="AA12" s="23"/>
       <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
+      <c r="AC12" s="23">
+        <v>2</v>
+      </c>
       <c r="AD12" s="26"/>
       <c r="AE12" s="26"/>
       <c r="AF12" s="23"/>
@@ -30374,7 +30837,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>13.25</v>
+        <v>15.25</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -30462,7 +30925,7 @@
       </c>
       <c r="AC36" s="79">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="AD36" s="78">
         <f t="shared" si="3"/>
@@ -30977,7 +31440,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Diagrama de casos de uso.png
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -36,7 +36,6 @@
     <definedName name="Print_Area" localSheetId="8">Sep!$A$1:$AR$37</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -305,7 +304,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="59">
   <si>
     <t>GP</t>
   </si>
@@ -479,6 +478,9 @@
   </si>
   <si>
     <t>Manual de administrador</t>
+  </si>
+  <si>
+    <t>Diagrama de casos de uso</t>
   </si>
 </sst>
 </file>
@@ -1958,7 +1960,7 @@
                   <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10.75</c:v>
@@ -2062,11 +2064,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49685632"/>
-        <c:axId val="49687552"/>
+        <c:axId val="146290176"/>
+        <c:axId val="146292096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49685632"/>
+        <c:axId val="146290176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2108,7 +2110,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49687552"/>
+        <c:crossAx val="146292096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2116,7 +2118,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49687552"/>
+        <c:axId val="146292096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2173,7 +2175,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49685632"/>
+        <c:crossAx val="146290176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2637,6 +2639,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3045,6 +3090,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3507,6 +3595,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3915,6 +4046,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4402,6 +4576,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4837,6 +5054,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5245,6 +5505,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6104,6 +6407,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6512,6 +6858,49 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="10" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6974,6 +7363,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7409,6 +7841,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -19050,7 +19525,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>40.75</v>
+        <v>41.05</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -19062,7 +19537,7 @@
       </c>
       <c r="J6" s="83">
         <f>Mar!G36</f>
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="K6" s="83">
         <f>Abr!G36</f>
@@ -22879,7 +23354,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23592,14 +24067,24 @@
     </row>
     <row r="10" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="B10" s="22">
+        <v>84</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2</v>
+      </c>
+      <c r="D10" s="23">
+        <v>57</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>58</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="23"/>
@@ -23623,7 +24108,9 @@
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
       <c r="AC10" s="26"/>
-      <c r="AD10" s="23"/>
+      <c r="AD10" s="23">
+        <v>0.3</v>
+      </c>
       <c r="AE10" s="23"/>
       <c r="AF10" s="23"/>
       <c r="AG10" s="23"/>
@@ -25161,7 +25648,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>10.3</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="1">SUM(H3:H35)</f>
@@ -25253,7 +25740,7 @@
       </c>
       <c r="AD36" s="79">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="AE36" s="79">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Cronograma_final.xls Esfuerzos Reales.xls Análisis esfuerzos reales vs estimados.doc Actualizada hoja de esfuerzos
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Alejandro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ene" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="61">
   <si>
     <t>GP</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>Diagrama de casos de uso</t>
+  </si>
+  <si>
+    <t>Reunion y reparto de tareas memoria final</t>
+  </si>
+  <si>
+    <t>Cronograma final, esfuerzos totales, planificación final</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1445,35 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF99CCFF"/>
+          <bgColor rgb="FF99CCFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1960,13 +1994,13 @@
                   <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.25</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2064,11 +2098,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="146290176"/>
-        <c:axId val="146292096"/>
+        <c:axId val="65546496"/>
+        <c:axId val="65548672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="146290176"/>
+        <c:axId val="65546496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2144,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146292096"/>
+        <c:crossAx val="65548672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2118,7 +2152,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146292096"/>
+        <c:axId val="65548672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2209,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146290176"/>
+        <c:crossAx val="65546496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2682,6 +2716,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3133,6 +3296,135 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -3638,6 +3930,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4089,6 +4510,135 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -4619,6 +5169,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5097,6 +5776,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5548,6 +6356,135 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6450,6 +7387,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6901,6 +7967,135 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -7406,6 +8601,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7884,6 +9208,135 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -19525,7 +20978,7 @@
       </c>
       <c r="G6" s="60">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>41.05</v>
+        <v>44.25</v>
       </c>
       <c r="H6" s="83">
         <f>Ene!G36</f>
@@ -19537,7 +20990,7 @@
       </c>
       <c r="J6" s="83">
         <f>Mar!G36</f>
-        <v>10.3</v>
+        <v>10</v>
       </c>
       <c r="K6" s="83">
         <f>Abr!G36</f>
@@ -19545,7 +20998,7 @@
       </c>
       <c r="L6" s="83">
         <f>May!G36</f>
-        <v>15.25</v>
+        <v>18.75</v>
       </c>
       <c r="M6" s="83">
         <f>Jun!G36</f>
@@ -23353,8 +24806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23579,7 +25032,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="16">
-        <f t="shared" ref="G3:G36" si="0">SUM(H3:AL3)</f>
+        <f>SUM(H3:AL3)</f>
         <v>1</v>
       </c>
       <c r="H3" s="17"/>
@@ -23651,7 +25104,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H4:AL4)</f>
         <v>0.5</v>
       </c>
       <c r="H4" s="26"/>
@@ -23723,7 +25176,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H5:AL5)</f>
         <v>1</v>
       </c>
       <c r="H5" s="26"/>
@@ -23795,7 +25248,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H6:AL6)</f>
         <v>2.5</v>
       </c>
       <c r="H6" s="26"/>
@@ -23867,7 +25320,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H7:AL7)</f>
         <v>2</v>
       </c>
       <c r="H7" s="26"/>
@@ -23939,7 +25392,7 @@
         <v>22</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H8:AL8)</f>
         <v>2</v>
       </c>
       <c r="H8" s="26"/>
@@ -24011,7 +25464,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H9:AL9)</f>
         <v>1</v>
       </c>
       <c r="H9" s="26"/>
@@ -24067,25 +25520,12 @@
     </row>
     <row r="10" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="22">
-        <v>84</v>
-      </c>
-      <c r="C10" s="23">
-        <v>2</v>
-      </c>
-      <c r="D10" s="23">
-        <v>57</v>
-      </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="16">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="26"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -24108,9 +25548,7 @@
       <c r="AA10" s="26"/>
       <c r="AB10" s="26"/>
       <c r="AC10" s="26"/>
-      <c r="AD10" s="23">
-        <v>0.3</v>
-      </c>
+      <c r="AD10" s="23"/>
       <c r="AE10" s="23"/>
       <c r="AF10" s="23"/>
       <c r="AG10" s="23"/>
@@ -24145,7 +25583,7 @@
       <c r="E11" s="24"/>
       <c r="F11" s="25"/>
       <c r="G11" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H11:AL11)</f>
         <v>0</v>
       </c>
       <c r="H11" s="26"/>
@@ -24205,7 +25643,7 @@
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
       <c r="G12" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H12:AL12)</f>
         <v>0</v>
       </c>
       <c r="H12" s="26"/>
@@ -24265,7 +25703,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H13:AL13)</f>
         <v>0</v>
       </c>
       <c r="H13" s="26"/>
@@ -24325,7 +25763,7 @@
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
       <c r="G14" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H14:AL14)</f>
         <v>0</v>
       </c>
       <c r="H14" s="26"/>
@@ -24385,7 +25823,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H15:AL15)</f>
         <v>0</v>
       </c>
       <c r="H15" s="26"/>
@@ -24445,7 +25883,7 @@
       <c r="E16" s="24"/>
       <c r="F16" s="25"/>
       <c r="G16" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H16:AL16)</f>
         <v>0</v>
       </c>
       <c r="H16" s="26"/>
@@ -24505,7 +25943,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="25"/>
       <c r="G17" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H17:AL17)</f>
         <v>0</v>
       </c>
       <c r="H17" s="26"/>
@@ -24565,7 +26003,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H18:AL18)</f>
         <v>0</v>
       </c>
       <c r="H18" s="26"/>
@@ -24625,7 +26063,7 @@
       <c r="E19" s="24"/>
       <c r="F19" s="25"/>
       <c r="G19" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H19:AL19)</f>
         <v>0</v>
       </c>
       <c r="H19" s="26"/>
@@ -24685,7 +26123,7 @@
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
       <c r="G20" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H20:AL20)</f>
         <v>0</v>
       </c>
       <c r="H20" s="26"/>
@@ -24745,7 +26183,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
       <c r="G21" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H21:AL21)</f>
         <v>0</v>
       </c>
       <c r="H21" s="26"/>
@@ -24805,7 +26243,7 @@
       <c r="E22" s="24"/>
       <c r="F22" s="25"/>
       <c r="G22" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H22:AL22)</f>
         <v>0</v>
       </c>
       <c r="H22" s="26"/>
@@ -24865,7 +26303,7 @@
       <c r="E23" s="24"/>
       <c r="F23" s="25"/>
       <c r="G23" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H23:AL23)</f>
         <v>0</v>
       </c>
       <c r="H23" s="26"/>
@@ -24925,7 +26363,7 @@
       <c r="E24" s="24"/>
       <c r="F24" s="25"/>
       <c r="G24" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H24:AL24)</f>
         <v>0</v>
       </c>
       <c r="H24" s="26"/>
@@ -24985,7 +26423,7 @@
       <c r="E25" s="24"/>
       <c r="F25" s="25"/>
       <c r="G25" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H25:AL25)</f>
         <v>0</v>
       </c>
       <c r="H25" s="26"/>
@@ -25045,7 +26483,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
       <c r="G26" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H26:AL26)</f>
         <v>0</v>
       </c>
       <c r="H26" s="26"/>
@@ -25105,7 +26543,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="25"/>
       <c r="G27" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H27:AL27)</f>
         <v>0</v>
       </c>
       <c r="H27" s="26"/>
@@ -25165,7 +26603,7 @@
       <c r="E28" s="24"/>
       <c r="F28" s="25"/>
       <c r="G28" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H28:AL28)</f>
         <v>0</v>
       </c>
       <c r="H28" s="26"/>
@@ -25225,7 +26663,7 @@
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
       <c r="G29" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H29:AL29)</f>
         <v>0</v>
       </c>
       <c r="H29" s="26"/>
@@ -25285,7 +26723,7 @@
       <c r="E30" s="24"/>
       <c r="F30" s="25"/>
       <c r="G30" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H30:AL30)</f>
         <v>0</v>
       </c>
       <c r="H30" s="26"/>
@@ -25345,7 +26783,7 @@
       <c r="E31" s="24"/>
       <c r="F31" s="25"/>
       <c r="G31" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H31:AL31)</f>
         <v>0</v>
       </c>
       <c r="H31" s="26"/>
@@ -25405,7 +26843,7 @@
       <c r="E32" s="24"/>
       <c r="F32" s="25"/>
       <c r="G32" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H32:AL32)</f>
         <v>0</v>
       </c>
       <c r="H32" s="26"/>
@@ -25465,7 +26903,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="G33" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H33:AL33)</f>
         <v>0</v>
       </c>
       <c r="H33" s="26"/>
@@ -25525,7 +26963,7 @@
       <c r="E34" s="24"/>
       <c r="F34" s="25"/>
       <c r="G34" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H34:AL34)</f>
         <v>0</v>
       </c>
       <c r="H34" s="26"/>
@@ -25585,7 +27023,7 @@
       <c r="E35" s="63"/>
       <c r="F35" s="64"/>
       <c r="G35" s="16">
-        <f t="shared" si="0"/>
+        <f>SUM(H35:AL35)</f>
         <v>0</v>
       </c>
       <c r="H35" s="69"/>
@@ -25647,131 +27085,131 @@
         <v>31</v>
       </c>
       <c r="G36" s="76">
-        <f t="shared" si="0"/>
-        <v>10.3</v>
+        <f>SUM(H36:AL36)</f>
+        <v>10</v>
       </c>
       <c r="H36" s="78">
-        <f t="shared" ref="H36:AL36" si="1">SUM(H3:H35)</f>
+        <f>SUM(H3:H35)</f>
         <v>0</v>
       </c>
       <c r="I36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(I3:I35)</f>
         <v>0</v>
       </c>
       <c r="J36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(J3:J35)</f>
         <v>0</v>
       </c>
       <c r="K36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(K3:K35)</f>
         <v>0</v>
       </c>
       <c r="L36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(L3:L35)</f>
         <v>0</v>
       </c>
       <c r="M36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(M3:M35)</f>
         <v>0</v>
       </c>
       <c r="N36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(N3:N35)</f>
         <v>0</v>
       </c>
       <c r="O36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(O3:O35)</f>
         <v>0</v>
       </c>
       <c r="P36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(P3:P35)</f>
         <v>1.5</v>
       </c>
       <c r="Q36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(Q3:Q35)</f>
         <v>0</v>
       </c>
       <c r="R36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(R3:R35)</f>
         <v>0</v>
       </c>
       <c r="S36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(S3:S35)</f>
         <v>7.5</v>
       </c>
       <c r="T36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(T3:T35)</f>
         <v>0</v>
       </c>
       <c r="U36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(U3:U35)</f>
         <v>0</v>
       </c>
       <c r="V36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(V3:V35)</f>
         <v>0</v>
       </c>
       <c r="W36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(W3:W35)</f>
         <v>0</v>
       </c>
       <c r="X36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(X3:X35)</f>
         <v>0</v>
       </c>
       <c r="Y36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(Y3:Y35)</f>
         <v>0</v>
       </c>
       <c r="Z36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(Z3:Z35)</f>
         <v>0</v>
       </c>
       <c r="AA36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AA3:AA35)</f>
         <v>0</v>
       </c>
       <c r="AB36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AB3:AB35)</f>
         <v>0</v>
       </c>
       <c r="AC36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AC3:AC35)</f>
         <v>0</v>
       </c>
       <c r="AD36" s="79">
-        <f t="shared" si="1"/>
-        <v>1.3</v>
+        <f>SUM(AD3:AD35)</f>
+        <v>1</v>
       </c>
       <c r="AE36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(AE3:AE35)</f>
         <v>0</v>
       </c>
       <c r="AF36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(AF3:AF35)</f>
         <v>0</v>
       </c>
       <c r="AG36" s="79">
-        <f t="shared" si="1"/>
+        <f>SUM(AG3:AG35)</f>
         <v>0</v>
       </c>
       <c r="AH36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AH3:AH35)</f>
         <v>0</v>
       </c>
       <c r="AI36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AI3:AI35)</f>
         <v>0</v>
       </c>
       <c r="AJ36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AJ3:AJ35)</f>
         <v>0</v>
       </c>
       <c r="AK36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AK3:AK35)</f>
         <v>0</v>
       </c>
       <c r="AL36" s="78">
-        <f t="shared" si="1"/>
+        <f>SUM(AL3:AL35)</f>
         <v>0</v>
       </c>
       <c r="AM36" s="1"/>
@@ -29009,8 +30447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH16" sqref="AH16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29671,33 +31109,33 @@
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
       <c r="V9" s="23"/>
-      <c r="W9" s="23">
+      <c r="W9" s="26">
         <v>2</v>
       </c>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="26">
+      <c r="X9" s="26"/>
+      <c r="Y9" s="23">
         <v>1</v>
       </c>
-      <c r="Z9" s="26"/>
+      <c r="Z9" s="23"/>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
       <c r="AD9" s="26"/>
       <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
       <c r="AH9" s="23"/>
       <c r="AI9" s="23"/>
       <c r="AJ9" s="23"/>
@@ -29802,9 +31240,11 @@
         <v>2</v>
       </c>
       <c r="D11" s="23">
-        <v>57</v>
-      </c>
-      <c r="E11" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="E11" s="24">
+        <v>6</v>
+      </c>
       <c r="F11" s="25" t="s">
         <v>56</v>
       </c>
@@ -29872,9 +31312,11 @@
         <v>2</v>
       </c>
       <c r="D12" s="23">
-        <v>57</v>
-      </c>
-      <c r="E12" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="E12" s="24">
+        <v>6</v>
+      </c>
       <c r="F12" s="25" t="s">
         <v>57</v>
       </c>
@@ -29935,14 +31377,24 @@
     </row>
     <row r="13" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="22">
+        <v>84</v>
+      </c>
+      <c r="C13" s="23">
+        <v>2</v>
+      </c>
+      <c r="D13" s="23">
+        <v>45</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>59</v>
+      </c>
       <c r="G13" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
@@ -29968,7 +31420,9 @@
       <c r="AC13" s="23"/>
       <c r="AD13" s="26"/>
       <c r="AE13" s="26"/>
-      <c r="AF13" s="23"/>
+      <c r="AF13" s="23">
+        <v>1</v>
+      </c>
       <c r="AG13" s="23"/>
       <c r="AH13" s="23"/>
       <c r="AI13" s="23"/>
@@ -29995,14 +31449,24 @@
     </row>
     <row r="14" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="B14" s="22">
+        <v>84</v>
+      </c>
+      <c r="C14" s="23">
+        <v>2</v>
+      </c>
+      <c r="D14" s="23">
+        <v>57</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>58</v>
+      </c>
       <c r="G14" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="26"/>
@@ -30026,7 +31490,9 @@
       <c r="AA14" s="23"/>
       <c r="AB14" s="23"/>
       <c r="AC14" s="23"/>
-      <c r="AD14" s="26"/>
+      <c r="AD14" s="26">
+        <v>0.5</v>
+      </c>
       <c r="AE14" s="26"/>
       <c r="AF14" s="23"/>
       <c r="AG14" s="23"/>
@@ -30055,14 +31521,22 @@
     </row>
     <row r="15" spans="1:55" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="22">
+        <v>84</v>
+      </c>
+      <c r="C15" s="23">
+        <v>2</v>
+      </c>
+      <c r="D15" s="23">
+        <v>57</v>
+      </c>
       <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="F15" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="26"/>
       <c r="I15" s="26"/>
@@ -30090,7 +31564,9 @@
       <c r="AE15" s="26"/>
       <c r="AF15" s="23"/>
       <c r="AG15" s="23"/>
-      <c r="AH15" s="23"/>
+      <c r="AH15" s="23">
+        <v>2</v>
+      </c>
       <c r="AI15" s="23"/>
       <c r="AJ15" s="23"/>
       <c r="AK15" s="26"/>
@@ -31324,7 +32800,7 @@
       </c>
       <c r="G36" s="76">
         <f t="shared" si="2"/>
-        <v>15.25</v>
+        <v>18.75</v>
       </c>
       <c r="H36" s="78">
         <f t="shared" ref="H36:AL36" si="3">SUM(H3:H35)</f>
@@ -31416,7 +32892,7 @@
       </c>
       <c r="AD36" s="78">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AE36" s="78">
         <f t="shared" si="3"/>
@@ -31424,7 +32900,7 @@
       </c>
       <c r="AF36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG36" s="79">
         <f t="shared" si="3"/>
@@ -31432,7 +32908,7 @@
       </c>
       <c r="AH36" s="79">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI36" s="79">
         <f t="shared" si="3"/>

</xml_diff>